<commit_message>
Final results with mapping v2
</commit_message>
<xml_diff>
--- a/data/cwe-cisIG1-mapping_v2.xlsx
+++ b/data/cwe-cisIG1-mapping_v2.xlsx
@@ -634,9 +634,9 @@
   <dimension ref="A1:AK26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="S1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="D26" sqref="D26"/>
+      <selection pane="topRight" activeCell="AA20" sqref="AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="6">
         <v>1</v>
@@ -967,10 +967,10 @@
         <v>0</v>
       </c>
       <c r="M4" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" s="6">
         <v>0</v>
@@ -1133,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="16">
         <v>0</v>
@@ -1157,13 +1157,13 @@
         <v>0</v>
       </c>
       <c r="O6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6" s="16">
         <v>0</v>
@@ -1178,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="V6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6" s="16">
         <v>0</v>
@@ -1199,10 +1199,10 @@
         <v>0</v>
       </c>
       <c r="AC6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -1691,7 +1691,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="6">
         <v>1</v>
@@ -1703,10 +1703,10 @@
         <v>0</v>
       </c>
       <c r="M12" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12" s="6">
         <v>1</v>
@@ -1961,13 +1961,13 @@
         <v>0</v>
       </c>
       <c r="G15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="16">
         <v>0</v>
       </c>
       <c r="I15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="6">
         <v>0</v>
@@ -1979,19 +1979,19 @@
         <v>0</v>
       </c>
       <c r="M15" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15" s="6">
         <v>0</v>
       </c>
       <c r="P15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15" s="16">
         <v>0</v>
@@ -2006,7 +2006,7 @@
         <v>0</v>
       </c>
       <c r="V15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W15" s="16">
         <v>0</v>
@@ -2027,10 +2027,10 @@
         <v>0</v>
       </c>
       <c r="AC15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -2053,7 +2053,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="16">
         <v>1</v>
@@ -2080,10 +2080,10 @@
         <v>0</v>
       </c>
       <c r="P16" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16" s="16">
         <v>0</v>
@@ -2098,7 +2098,7 @@
         <v>0</v>
       </c>
       <c r="V16" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W16" s="16">
         <v>0</v>
@@ -2119,10 +2119,10 @@
         <v>0</v>
       </c>
       <c r="AC16" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD16" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.3">
@@ -2169,7 +2169,7 @@
         <v>0</v>
       </c>
       <c r="O17" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="16">
         <v>0</v>
@@ -2421,7 +2421,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="16">
         <v>1</v>
@@ -2436,7 +2436,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" s="16">
         <v>0</v>
@@ -2445,13 +2445,13 @@
         <v>0</v>
       </c>
       <c r="O20" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R20" s="16">
         <v>0</v>
@@ -2460,13 +2460,13 @@
         <v>0</v>
       </c>
       <c r="T20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20" s="16">
         <v>0</v>
@@ -2478,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="Z20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA20" s="16">
         <v>1</v>
@@ -2487,10 +2487,10 @@
         <v>0</v>
       </c>
       <c r="AC20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
@@ -2789,7 +2789,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="16">
         <v>0</v>
@@ -2816,10 +2816,10 @@
         <v>0</v>
       </c>
       <c r="P24" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24" s="16">
         <v>1</v>
@@ -2834,7 +2834,7 @@
         <v>0</v>
       </c>
       <c r="V24" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W24" s="16">
         <v>1</v>
@@ -2855,10 +2855,10 @@
         <v>0</v>
       </c>
       <c r="AC24" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD24" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.3">
@@ -2979,7 +2979,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="6">
         <v>0</v>
@@ -2991,10 +2991,10 @@
         <v>0</v>
       </c>
       <c r="M26" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O26" s="6">
         <v>0</v>

</xml_diff>